<commit_message>
Integrated all the scenarios.
1.Included Request Id update in the scripts.

2.Create save as draft Issue fix.

3.Global Data for Material updated.

4.Approval flow added for duplicate and non duplicate flows.

5.Mendix Testplan sheet updated.

6.JDE scripts updated for Excel inputs.
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SatishKumarSundaramo\git\Mendix_New\Mendix\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190FFA13-8E62-43F3-87E1-8E71B919C4EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1084400-95E7-4A61-A414-FCE43397F8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,19 @@
     <sheet name="Scripts" sheetId="2" r:id="rId2"/>
     <sheet name="Environment" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
   <si>
     <t>S.NO</t>
   </si>
@@ -75,9 +82,6 @@
     <t>1377436</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -268,13 +272,46 @@
   </si>
   <si>
     <t>1402111</t>
+  </si>
+  <si>
+    <t>30007590</t>
+  </si>
+  <si>
+    <t>30007783</t>
+  </si>
+  <si>
+    <t>161144</t>
+  </si>
+  <si>
+    <t>1415905</t>
+  </si>
+  <si>
+    <t>Create_Material_Global_and_Local_for_JDE</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1415919</t>
+  </si>
+  <si>
+    <t>502837</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Create_Vendor_with_Questionnaire_only_Global</t>
+  </si>
+  <si>
+    <t>SG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Mic Shell Dlg"/>
@@ -282,12 +319,6 @@
     <font>
       <sz val="11"/>
       <name val="Mic Shell Dlg"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -321,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -330,9 +361,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -677,37 +705,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IX6"/>
+  <dimension ref="A1:IX8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="1" customWidth="1"/>
-    <col min="17" max="258" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="69.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="258" width="9.140625" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:258" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -719,16 +746,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -753,20 +780,20 @@
       </c>
     </row>
     <row r="2" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>67</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
@@ -775,42 +802,45 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2">
-        <v>161144</v>
-      </c>
-      <c r="L2" s="2">
-        <v>30007589</v>
-      </c>
-      <c r="M2" s="2">
-        <v>30007782</v>
+      <c r="K2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>68</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>4</v>
@@ -819,42 +849,42 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2">
-        <v>161144</v>
-      </c>
-      <c r="L3" s="2">
-        <v>30007590</v>
-      </c>
-      <c r="M3" s="2">
-        <v>30007783</v>
+      <c r="K3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>16</v>
@@ -866,45 +896,45 @@
         <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="2">
-        <v>161144</v>
-      </c>
-      <c r="L4" s="2">
-        <v>30007590</v>
-      </c>
-      <c r="M4" s="2">
-        <v>30007783</v>
+      <c r="K4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:258" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="5" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>4</v>
@@ -913,317 +943,656 @@
         <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="2">
-        <v>161144</v>
-      </c>
-      <c r="L5" s="2">
-        <v>30007590</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="K5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:258" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:258" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="7">
         <v>30007783</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:258" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="N7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="8"/>
+      <c r="AR7" s="8"/>
+      <c r="AS7" s="8"/>
+      <c r="AT7" s="8"/>
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="8"/>
+      <c r="AW7" s="8"/>
+      <c r="AX7" s="8"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="8"/>
+      <c r="BA7" s="8"/>
+      <c r="BB7" s="8"/>
+      <c r="BC7" s="8"/>
+      <c r="BD7" s="8"/>
+      <c r="BE7" s="8"/>
+      <c r="BF7" s="8"/>
+      <c r="BG7" s="8"/>
+      <c r="BH7" s="8"/>
+      <c r="BI7" s="8"/>
+      <c r="BJ7" s="8"/>
+      <c r="BK7" s="8"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="8"/>
+      <c r="BQ7" s="8"/>
+      <c r="BR7" s="8"/>
+      <c r="BS7" s="8"/>
+      <c r="BT7" s="8"/>
+      <c r="BU7" s="8"/>
+      <c r="BV7" s="8"/>
+      <c r="BW7" s="8"/>
+      <c r="BX7" s="8"/>
+      <c r="BY7" s="8"/>
+      <c r="BZ7" s="8"/>
+      <c r="CA7" s="8"/>
+      <c r="CB7" s="8"/>
+      <c r="CC7" s="8"/>
+      <c r="CD7" s="8"/>
+      <c r="CE7" s="8"/>
+      <c r="CF7" s="8"/>
+      <c r="CG7" s="8"/>
+      <c r="CH7" s="8"/>
+      <c r="CI7" s="8"/>
+      <c r="CJ7" s="8"/>
+      <c r="CK7" s="8"/>
+      <c r="CL7" s="8"/>
+      <c r="CM7" s="8"/>
+      <c r="CN7" s="8"/>
+      <c r="CO7" s="8"/>
+      <c r="CP7" s="8"/>
+      <c r="CQ7" s="8"/>
+      <c r="CR7" s="8"/>
+      <c r="CS7" s="8"/>
+      <c r="CT7" s="8"/>
+      <c r="CU7" s="8"/>
+      <c r="CV7" s="8"/>
+      <c r="CW7" s="8"/>
+      <c r="CX7" s="8"/>
+      <c r="CY7" s="8"/>
+      <c r="CZ7" s="8"/>
+      <c r="DA7" s="8"/>
+      <c r="DB7" s="8"/>
+      <c r="DC7" s="8"/>
+      <c r="DD7" s="8"/>
+      <c r="DE7" s="8"/>
+      <c r="DF7" s="8"/>
+      <c r="DG7" s="8"/>
+      <c r="DH7" s="8"/>
+      <c r="DI7" s="8"/>
+      <c r="DJ7" s="8"/>
+      <c r="DK7" s="8"/>
+      <c r="DL7" s="8"/>
+      <c r="DM7" s="8"/>
+      <c r="DN7" s="8"/>
+      <c r="DO7" s="8"/>
+      <c r="DP7" s="8"/>
+      <c r="DQ7" s="8"/>
+      <c r="DR7" s="8"/>
+      <c r="DS7" s="8"/>
+      <c r="DT7" s="8"/>
+      <c r="DU7" s="8"/>
+      <c r="DV7" s="8"/>
+      <c r="DW7" s="8"/>
+      <c r="DX7" s="8"/>
+      <c r="DY7" s="8"/>
+      <c r="DZ7" s="8"/>
+      <c r="EA7" s="8"/>
+      <c r="EB7" s="8"/>
+      <c r="EC7" s="8"/>
+      <c r="ED7" s="8"/>
+      <c r="EE7" s="8"/>
+      <c r="EF7" s="8"/>
+      <c r="EG7" s="8"/>
+      <c r="EH7" s="8"/>
+      <c r="EI7" s="8"/>
+      <c r="EJ7" s="8"/>
+      <c r="EK7" s="8"/>
+      <c r="EL7" s="8"/>
+      <c r="EM7" s="8"/>
+      <c r="EN7" s="8"/>
+      <c r="EO7" s="8"/>
+      <c r="EP7" s="8"/>
+      <c r="EQ7" s="8"/>
+      <c r="ER7" s="8"/>
+      <c r="ES7" s="8"/>
+      <c r="ET7" s="8"/>
+      <c r="EU7" s="8"/>
+      <c r="EV7" s="8"/>
+      <c r="EW7" s="8"/>
+      <c r="EX7" s="8"/>
+      <c r="EY7" s="8"/>
+      <c r="EZ7" s="8"/>
+      <c r="FA7" s="8"/>
+      <c r="FB7" s="8"/>
+      <c r="FC7" s="8"/>
+      <c r="FD7" s="8"/>
+      <c r="FE7" s="8"/>
+      <c r="FF7" s="8"/>
+      <c r="FG7" s="8"/>
+      <c r="FH7" s="8"/>
+      <c r="FI7" s="8"/>
+      <c r="FJ7" s="8"/>
+      <c r="FK7" s="8"/>
+      <c r="FL7" s="8"/>
+      <c r="FM7" s="8"/>
+      <c r="FN7" s="8"/>
+      <c r="FO7" s="8"/>
+      <c r="FP7" s="8"/>
+      <c r="FQ7" s="8"/>
+      <c r="FR7" s="8"/>
+      <c r="FS7" s="8"/>
+      <c r="FT7" s="8"/>
+      <c r="FU7" s="8"/>
+      <c r="FV7" s="8"/>
+      <c r="FW7" s="8"/>
+      <c r="FX7" s="8"/>
+      <c r="FY7" s="8"/>
+      <c r="FZ7" s="8"/>
+      <c r="GA7" s="8"/>
+      <c r="GB7" s="8"/>
+      <c r="GC7" s="8"/>
+      <c r="GD7" s="8"/>
+      <c r="GE7" s="8"/>
+      <c r="GF7" s="8"/>
+      <c r="GG7" s="8"/>
+      <c r="GH7" s="8"/>
+      <c r="GI7" s="8"/>
+      <c r="GJ7" s="8"/>
+      <c r="GK7" s="8"/>
+      <c r="GL7" s="8"/>
+      <c r="GM7" s="8"/>
+      <c r="GN7" s="8"/>
+      <c r="GO7" s="8"/>
+      <c r="GP7" s="8"/>
+      <c r="GQ7" s="8"/>
+      <c r="GR7" s="8"/>
+      <c r="GS7" s="8"/>
+      <c r="GT7" s="8"/>
+      <c r="GU7" s="8"/>
+      <c r="GV7" s="8"/>
+      <c r="GW7" s="8"/>
+      <c r="GX7" s="8"/>
+      <c r="GY7" s="8"/>
+      <c r="GZ7" s="8"/>
+      <c r="HA7" s="8"/>
+      <c r="HB7" s="8"/>
+      <c r="HC7" s="8"/>
+      <c r="HD7" s="8"/>
+      <c r="HE7" s="8"/>
+      <c r="HF7" s="8"/>
+      <c r="HG7" s="8"/>
+      <c r="HH7" s="8"/>
+      <c r="HI7" s="8"/>
+      <c r="HJ7" s="8"/>
+      <c r="HK7" s="8"/>
+      <c r="HL7" s="8"/>
+      <c r="HM7" s="8"/>
+      <c r="HN7" s="8"/>
+      <c r="HO7" s="8"/>
+      <c r="HP7" s="8"/>
+      <c r="HQ7" s="8"/>
+      <c r="HR7" s="8"/>
+      <c r="HS7" s="8"/>
+      <c r="HT7" s="8"/>
+      <c r="HU7" s="8"/>
+      <c r="HV7" s="8"/>
+      <c r="HW7" s="8"/>
+      <c r="HX7" s="8"/>
+      <c r="HY7" s="8"/>
+      <c r="HZ7" s="8"/>
+      <c r="IA7" s="8"/>
+      <c r="IB7" s="8"/>
+      <c r="IC7" s="8"/>
+      <c r="ID7" s="8"/>
+      <c r="IE7" s="8"/>
+      <c r="IF7" s="8"/>
+      <c r="IG7" s="8"/>
+      <c r="IH7" s="8"/>
+      <c r="II7" s="8"/>
+      <c r="IJ7" s="8"/>
+      <c r="IK7" s="8"/>
+      <c r="IL7" s="8"/>
+      <c r="IM7" s="8"/>
+      <c r="IN7" s="8"/>
+      <c r="IO7" s="8"/>
+      <c r="IP7" s="8"/>
+      <c r="IQ7" s="8"/>
+      <c r="IR7" s="8"/>
+      <c r="IS7" s="8"/>
+      <c r="IT7" s="8"/>
+      <c r="IU7" s="8"/>
+      <c r="IV7" s="8"/>
+      <c r="IW7" s="8"/>
+      <c r="IX7" s="8"/>
+    </row>
+    <row r="8" spans="1:258" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="F8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="7">
+        <v>30007783</v>
+      </c>
+      <c r="N8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="10">
-        <v>30007590</v>
-      </c>
-      <c r="M6" s="10">
-        <v>30007783</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-      <c r="AU6" s="9"/>
-      <c r="AV6" s="9"/>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="9"/>
-      <c r="AY6" s="9"/>
-      <c r="AZ6" s="9"/>
-      <c r="BA6" s="9"/>
-      <c r="BB6" s="9"/>
-      <c r="BC6" s="9"/>
-      <c r="BD6" s="9"/>
-      <c r="BE6" s="9"/>
-      <c r="BF6" s="9"/>
-      <c r="BG6" s="9"/>
-      <c r="BH6" s="9"/>
-      <c r="BI6" s="9"/>
-      <c r="BJ6" s="9"/>
-      <c r="BK6" s="9"/>
-      <c r="BL6" s="9"/>
-      <c r="BM6" s="9"/>
-      <c r="BN6" s="9"/>
-      <c r="BO6" s="9"/>
-      <c r="BP6" s="9"/>
-      <c r="BQ6" s="9"/>
-      <c r="BR6" s="9"/>
-      <c r="BS6" s="9"/>
-      <c r="BT6" s="9"/>
-      <c r="BU6" s="9"/>
-      <c r="BV6" s="9"/>
-      <c r="BW6" s="9"/>
-      <c r="BX6" s="9"/>
-      <c r="BY6" s="9"/>
-      <c r="BZ6" s="9"/>
-      <c r="CA6" s="9"/>
-      <c r="CB6" s="9"/>
-      <c r="CC6" s="9"/>
-      <c r="CD6" s="9"/>
-      <c r="CE6" s="9"/>
-      <c r="CF6" s="9"/>
-      <c r="CG6" s="9"/>
-      <c r="CH6" s="9"/>
-      <c r="CI6" s="9"/>
-      <c r="CJ6" s="9"/>
-      <c r="CK6" s="9"/>
-      <c r="CL6" s="9"/>
-      <c r="CM6" s="9"/>
-      <c r="CN6" s="9"/>
-      <c r="CO6" s="9"/>
-      <c r="CP6" s="9"/>
-      <c r="CQ6" s="9"/>
-      <c r="CR6" s="9"/>
-      <c r="CS6" s="9"/>
-      <c r="CT6" s="9"/>
-      <c r="CU6" s="9"/>
-      <c r="CV6" s="9"/>
-      <c r="CW6" s="9"/>
-      <c r="CX6" s="9"/>
-      <c r="CY6" s="9"/>
-      <c r="CZ6" s="9"/>
-      <c r="DA6" s="9"/>
-      <c r="DB6" s="9"/>
-      <c r="DC6" s="9"/>
-      <c r="DD6" s="9"/>
-      <c r="DE6" s="9"/>
-      <c r="DF6" s="9"/>
-      <c r="DG6" s="9"/>
-      <c r="DH6" s="9"/>
-      <c r="DI6" s="9"/>
-      <c r="DJ6" s="9"/>
-      <c r="DK6" s="9"/>
-      <c r="DL6" s="9"/>
-      <c r="DM6" s="9"/>
-      <c r="DN6" s="9"/>
-      <c r="DO6" s="9"/>
-      <c r="DP6" s="9"/>
-      <c r="DQ6" s="9"/>
-      <c r="DR6" s="9"/>
-      <c r="DS6" s="9"/>
-      <c r="DT6" s="9"/>
-      <c r="DU6" s="9"/>
-      <c r="DV6" s="9"/>
-      <c r="DW6" s="9"/>
-      <c r="DX6" s="9"/>
-      <c r="DY6" s="9"/>
-      <c r="DZ6" s="9"/>
-      <c r="EA6" s="9"/>
-      <c r="EB6" s="9"/>
-      <c r="EC6" s="9"/>
-      <c r="ED6" s="9"/>
-      <c r="EE6" s="9"/>
-      <c r="EF6" s="9"/>
-      <c r="EG6" s="9"/>
-      <c r="EH6" s="9"/>
-      <c r="EI6" s="9"/>
-      <c r="EJ6" s="9"/>
-      <c r="EK6" s="9"/>
-      <c r="EL6" s="9"/>
-      <c r="EM6" s="9"/>
-      <c r="EN6" s="9"/>
-      <c r="EO6" s="9"/>
-      <c r="EP6" s="9"/>
-      <c r="EQ6" s="9"/>
-      <c r="ER6" s="9"/>
-      <c r="ES6" s="9"/>
-      <c r="ET6" s="9"/>
-      <c r="EU6" s="9"/>
-      <c r="EV6" s="9"/>
-      <c r="EW6" s="9"/>
-      <c r="EX6" s="9"/>
-      <c r="EY6" s="9"/>
-      <c r="EZ6" s="9"/>
-      <c r="FA6" s="9"/>
-      <c r="FB6" s="9"/>
-      <c r="FC6" s="9"/>
-      <c r="FD6" s="9"/>
-      <c r="FE6" s="9"/>
-      <c r="FF6" s="9"/>
-      <c r="FG6" s="9"/>
-      <c r="FH6" s="9"/>
-      <c r="FI6" s="9"/>
-      <c r="FJ6" s="9"/>
-      <c r="FK6" s="9"/>
-      <c r="FL6" s="9"/>
-      <c r="FM6" s="9"/>
-      <c r="FN6" s="9"/>
-      <c r="FO6" s="9"/>
-      <c r="FP6" s="9"/>
-      <c r="FQ6" s="9"/>
-      <c r="FR6" s="9"/>
-      <c r="FS6" s="9"/>
-      <c r="FT6" s="9"/>
-      <c r="FU6" s="9"/>
-      <c r="FV6" s="9"/>
-      <c r="FW6" s="9"/>
-      <c r="FX6" s="9"/>
-      <c r="FY6" s="9"/>
-      <c r="FZ6" s="9"/>
-      <c r="GA6" s="9"/>
-      <c r="GB6" s="9"/>
-      <c r="GC6" s="9"/>
-      <c r="GD6" s="9"/>
-      <c r="GE6" s="9"/>
-      <c r="GF6" s="9"/>
-      <c r="GG6" s="9"/>
-      <c r="GH6" s="9"/>
-      <c r="GI6" s="9"/>
-      <c r="GJ6" s="9"/>
-      <c r="GK6" s="9"/>
-      <c r="GL6" s="9"/>
-      <c r="GM6" s="9"/>
-      <c r="GN6" s="9"/>
-      <c r="GO6" s="9"/>
-      <c r="GP6" s="9"/>
-      <c r="GQ6" s="9"/>
-      <c r="GR6" s="9"/>
-      <c r="GS6" s="9"/>
-      <c r="GT6" s="9"/>
-      <c r="GU6" s="9"/>
-      <c r="GV6" s="9"/>
-      <c r="GW6" s="9"/>
-      <c r="GX6" s="9"/>
-      <c r="GY6" s="9"/>
-      <c r="GZ6" s="9"/>
-      <c r="HA6" s="9"/>
-      <c r="HB6" s="9"/>
-      <c r="HC6" s="9"/>
-      <c r="HD6" s="9"/>
-      <c r="HE6" s="9"/>
-      <c r="HF6" s="9"/>
-      <c r="HG6" s="9"/>
-      <c r="HH6" s="9"/>
-      <c r="HI6" s="9"/>
-      <c r="HJ6" s="9"/>
-      <c r="HK6" s="9"/>
-      <c r="HL6" s="9"/>
-      <c r="HM6" s="9"/>
-      <c r="HN6" s="9"/>
-      <c r="HO6" s="9"/>
-      <c r="HP6" s="9"/>
-      <c r="HQ6" s="9"/>
-      <c r="HR6" s="9"/>
-      <c r="HS6" s="9"/>
-      <c r="HT6" s="9"/>
-      <c r="HU6" s="9"/>
-      <c r="HV6" s="9"/>
-      <c r="HW6" s="9"/>
-      <c r="HX6" s="9"/>
-      <c r="HY6" s="9"/>
-      <c r="HZ6" s="9"/>
-      <c r="IA6" s="9"/>
-      <c r="IB6" s="9"/>
-      <c r="IC6" s="9"/>
-      <c r="ID6" s="9"/>
-      <c r="IE6" s="9"/>
-      <c r="IF6" s="9"/>
-      <c r="IG6" s="9"/>
-      <c r="IH6" s="9"/>
-      <c r="II6" s="9"/>
-      <c r="IJ6" s="9"/>
-      <c r="IK6" s="9"/>
-      <c r="IL6" s="9"/>
-      <c r="IM6" s="9"/>
-      <c r="IN6" s="9"/>
-      <c r="IO6" s="9"/>
-      <c r="IP6" s="9"/>
-      <c r="IQ6" s="9"/>
-      <c r="IR6" s="9"/>
-      <c r="IS6" s="9"/>
-      <c r="IT6" s="9"/>
-      <c r="IU6" s="9"/>
-      <c r="IV6" s="9"/>
-      <c r="IW6" s="9"/>
-      <c r="IX6" s="9"/>
+      <c r="O8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="8"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8"/>
+      <c r="BA8" s="8"/>
+      <c r="BB8" s="8"/>
+      <c r="BC8" s="8"/>
+      <c r="BD8" s="8"/>
+      <c r="BE8" s="8"/>
+      <c r="BF8" s="8"/>
+      <c r="BG8" s="8"/>
+      <c r="BH8" s="8"/>
+      <c r="BI8" s="8"/>
+      <c r="BJ8" s="8"/>
+      <c r="BK8" s="8"/>
+      <c r="BL8" s="8"/>
+      <c r="BM8" s="8"/>
+      <c r="BN8" s="8"/>
+      <c r="BO8" s="8"/>
+      <c r="BP8" s="8"/>
+      <c r="BQ8" s="8"/>
+      <c r="BR8" s="8"/>
+      <c r="BS8" s="8"/>
+      <c r="BT8" s="8"/>
+      <c r="BU8" s="8"/>
+      <c r="BV8" s="8"/>
+      <c r="BW8" s="8"/>
+      <c r="BX8" s="8"/>
+      <c r="BY8" s="8"/>
+      <c r="BZ8" s="8"/>
+      <c r="CA8" s="8"/>
+      <c r="CB8" s="8"/>
+      <c r="CC8" s="8"/>
+      <c r="CD8" s="8"/>
+      <c r="CE8" s="8"/>
+      <c r="CF8" s="8"/>
+      <c r="CG8" s="8"/>
+      <c r="CH8" s="8"/>
+      <c r="CI8" s="8"/>
+      <c r="CJ8" s="8"/>
+      <c r="CK8" s="8"/>
+      <c r="CL8" s="8"/>
+      <c r="CM8" s="8"/>
+      <c r="CN8" s="8"/>
+      <c r="CO8" s="8"/>
+      <c r="CP8" s="8"/>
+      <c r="CQ8" s="8"/>
+      <c r="CR8" s="8"/>
+      <c r="CS8" s="8"/>
+      <c r="CT8" s="8"/>
+      <c r="CU8" s="8"/>
+      <c r="CV8" s="8"/>
+      <c r="CW8" s="8"/>
+      <c r="CX8" s="8"/>
+      <c r="CY8" s="8"/>
+      <c r="CZ8" s="8"/>
+      <c r="DA8" s="8"/>
+      <c r="DB8" s="8"/>
+      <c r="DC8" s="8"/>
+      <c r="DD8" s="8"/>
+      <c r="DE8" s="8"/>
+      <c r="DF8" s="8"/>
+      <c r="DG8" s="8"/>
+      <c r="DH8" s="8"/>
+      <c r="DI8" s="8"/>
+      <c r="DJ8" s="8"/>
+      <c r="DK8" s="8"/>
+      <c r="DL8" s="8"/>
+      <c r="DM8" s="8"/>
+      <c r="DN8" s="8"/>
+      <c r="DO8" s="8"/>
+      <c r="DP8" s="8"/>
+      <c r="DQ8" s="8"/>
+      <c r="DR8" s="8"/>
+      <c r="DS8" s="8"/>
+      <c r="DT8" s="8"/>
+      <c r="DU8" s="8"/>
+      <c r="DV8" s="8"/>
+      <c r="DW8" s="8"/>
+      <c r="DX8" s="8"/>
+      <c r="DY8" s="8"/>
+      <c r="DZ8" s="8"/>
+      <c r="EA8" s="8"/>
+      <c r="EB8" s="8"/>
+      <c r="EC8" s="8"/>
+      <c r="ED8" s="8"/>
+      <c r="EE8" s="8"/>
+      <c r="EF8" s="8"/>
+      <c r="EG8" s="8"/>
+      <c r="EH8" s="8"/>
+      <c r="EI8" s="8"/>
+      <c r="EJ8" s="8"/>
+      <c r="EK8" s="8"/>
+      <c r="EL8" s="8"/>
+      <c r="EM8" s="8"/>
+      <c r="EN8" s="8"/>
+      <c r="EO8" s="8"/>
+      <c r="EP8" s="8"/>
+      <c r="EQ8" s="8"/>
+      <c r="ER8" s="8"/>
+      <c r="ES8" s="8"/>
+      <c r="ET8" s="8"/>
+      <c r="EU8" s="8"/>
+      <c r="EV8" s="8"/>
+      <c r="EW8" s="8"/>
+      <c r="EX8" s="8"/>
+      <c r="EY8" s="8"/>
+      <c r="EZ8" s="8"/>
+      <c r="FA8" s="8"/>
+      <c r="FB8" s="8"/>
+      <c r="FC8" s="8"/>
+      <c r="FD8" s="8"/>
+      <c r="FE8" s="8"/>
+      <c r="FF8" s="8"/>
+      <c r="FG8" s="8"/>
+      <c r="FH8" s="8"/>
+      <c r="FI8" s="8"/>
+      <c r="FJ8" s="8"/>
+      <c r="FK8" s="8"/>
+      <c r="FL8" s="8"/>
+      <c r="FM8" s="8"/>
+      <c r="FN8" s="8"/>
+      <c r="FO8" s="8"/>
+      <c r="FP8" s="8"/>
+      <c r="FQ8" s="8"/>
+      <c r="FR8" s="8"/>
+      <c r="FS8" s="8"/>
+      <c r="FT8" s="8"/>
+      <c r="FU8" s="8"/>
+      <c r="FV8" s="8"/>
+      <c r="FW8" s="8"/>
+      <c r="FX8" s="8"/>
+      <c r="FY8" s="8"/>
+      <c r="FZ8" s="8"/>
+      <c r="GA8" s="8"/>
+      <c r="GB8" s="8"/>
+      <c r="GC8" s="8"/>
+      <c r="GD8" s="8"/>
+      <c r="GE8" s="8"/>
+      <c r="GF8" s="8"/>
+      <c r="GG8" s="8"/>
+      <c r="GH8" s="8"/>
+      <c r="GI8" s="8"/>
+      <c r="GJ8" s="8"/>
+      <c r="GK8" s="8"/>
+      <c r="GL8" s="8"/>
+      <c r="GM8" s="8"/>
+      <c r="GN8" s="8"/>
+      <c r="GO8" s="8"/>
+      <c r="GP8" s="8"/>
+      <c r="GQ8" s="8"/>
+      <c r="GR8" s="8"/>
+      <c r="GS8" s="8"/>
+      <c r="GT8" s="8"/>
+      <c r="GU8" s="8"/>
+      <c r="GV8" s="8"/>
+      <c r="GW8" s="8"/>
+      <c r="GX8" s="8"/>
+      <c r="GY8" s="8"/>
+      <c r="GZ8" s="8"/>
+      <c r="HA8" s="8"/>
+      <c r="HB8" s="8"/>
+      <c r="HC8" s="8"/>
+      <c r="HD8" s="8"/>
+      <c r="HE8" s="8"/>
+      <c r="HF8" s="8"/>
+      <c r="HG8" s="8"/>
+      <c r="HH8" s="8"/>
+      <c r="HI8" s="8"/>
+      <c r="HJ8" s="8"/>
+      <c r="HK8" s="8"/>
+      <c r="HL8" s="8"/>
+      <c r="HM8" s="8"/>
+      <c r="HN8" s="8"/>
+      <c r="HO8" s="8"/>
+      <c r="HP8" s="8"/>
+      <c r="HQ8" s="8"/>
+      <c r="HR8" s="8"/>
+      <c r="HS8" s="8"/>
+      <c r="HT8" s="8"/>
+      <c r="HU8" s="8"/>
+      <c r="HV8" s="8"/>
+      <c r="HW8" s="8"/>
+      <c r="HX8" s="8"/>
+      <c r="HY8" s="8"/>
+      <c r="HZ8" s="8"/>
+      <c r="IA8" s="8"/>
+      <c r="IB8" s="8"/>
+      <c r="IC8" s="8"/>
+      <c r="ID8" s="8"/>
+      <c r="IE8" s="8"/>
+      <c r="IF8" s="8"/>
+      <c r="IG8" s="8"/>
+      <c r="IH8" s="8"/>
+      <c r="II8" s="8"/>
+      <c r="IJ8" s="8"/>
+      <c r="IK8" s="8"/>
+      <c r="IL8" s="8"/>
+      <c r="IM8" s="8"/>
+      <c r="IN8" s="8"/>
+      <c r="IO8" s="8"/>
+      <c r="IP8" s="8"/>
+      <c r="IQ8" s="8"/>
+      <c r="IR8" s="8"/>
+      <c r="IS8" s="8"/>
+      <c r="IT8" s="8"/>
+      <c r="IU8" s="8"/>
+      <c r="IV8" s="8"/>
+      <c r="IW8" s="8"/>
+      <c r="IX8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1246,31 +1615,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="55" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="55" style="1" customWidth="1"/>
-    <col min="6" max="254" width="9.140625" style="1" customWidth="1"/>
-    <col min="255" max="255" width="4.85546875" style="1" customWidth="1"/>
-    <col min="256" max="256" width="55" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="254" width="9.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="255" max="255" width="4.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="256" max="256" width="55" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,84 +1647,84 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1374,43 +1743,43 @@
   <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="123.140625" style="3" customWidth="1"/>
-    <col min="3" max="256" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="123.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="256" width="9.140625" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3">
         <v>30</v>
@@ -1418,7 +1787,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3">
         <v>30</v>
@@ -1426,7 +1795,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3">
         <v>30</v>
@@ -1434,7 +1803,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -1442,7 +1811,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -1450,7 +1819,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -1458,7 +1827,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -1466,7 +1835,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3">
         <v>5</v>
@@ -1474,7 +1843,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3">
         <v>6</v>
@@ -1482,63 +1851,63 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>14</v>
@@ -1546,10 +1915,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Click Flag for deletion button method is added
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SatishKumarSundaramo\git\Mendix_New\Mendix\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A83225D-E457-4C23-AE48-ABACDAA8EE9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4FD37E-38F5-4980-AA71-9C543F55B10B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="330">
   <si>
     <t>S.NO</t>
   </si>
@@ -798,9 +798,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>502869</t>
-  </si>
-  <si>
     <t>GBDA</t>
   </si>
   <si>
@@ -882,9 +879,6 @@
     <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_and_Bank_JDE</t>
   </si>
   <si>
-    <t>502870</t>
-  </si>
-  <si>
     <t>S.No</t>
   </si>
   <si>
@@ -1012,9 +1006,6 @@
   </si>
   <si>
     <t>Production | Raw material, ingredient or processing aid</t>
-  </si>
-  <si>
-    <t>1416842</t>
   </si>
   <si>
     <t>502871</t>
@@ -1027,7 +1018,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1418,27 +1408,27 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="75.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="11.140625" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="13.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="10.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
-    <col min="17" max="256" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="9.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="75.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="256" width="9.140625" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2222,390 +2212,390 @@
         <v>257</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:255" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>257</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="O3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:255" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>257</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="O4" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:255" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>257</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="O5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:255" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>257</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="O6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>257</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="M7" s="3">
         <v>30007783</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="M8" s="3">
         <v>30007783</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>257</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M9" s="3">
         <v>30007783</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2629,31 +2619,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="55.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="24.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="55.0" collapsed="true"/>
-    <col min="6" max="254" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="255" max="255" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="256" max="256" customWidth="true" style="1" width="55.0" collapsed="true"/>
+    <col min="1" max="1" width="4.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="254" width="9.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="255" max="255" width="4.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="256" max="256" width="55" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2661,84 +2651,84 @@
         <v>255</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2762,30 +2752,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="123.140625" collapsed="true"/>
-    <col min="3" max="256" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="123.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="256" width="9.140625" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>257</v>
@@ -2793,7 +2783,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B4" s="4">
         <v>30</v>
@@ -2801,7 +2791,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B5" s="4">
         <v>30</v>
@@ -2809,7 +2799,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B6" s="4">
         <v>30</v>
@@ -2817,7 +2807,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -2825,7 +2815,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -2833,7 +2823,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
@@ -2841,7 +2831,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B10" s="4">
         <v>3</v>
@@ -2849,7 +2839,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B11" s="4">
         <v>5</v>
@@ -2857,7 +2847,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B12" s="4">
         <v>6</v>
@@ -2865,39 +2855,39 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>238</v>
@@ -2905,23 +2895,23 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>56</v>
@@ -2929,10 +2919,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>